<commit_message>
Adding Redes sociales testcases
</commit_message>
<xml_diff>
--- a/solvex_testcases.xlsx
+++ b/solvex_testcases.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rafael Mejia\solvex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544D0299-8E9B-4269-99BB-0E67EF0D8762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D15886-1826-41CC-B489-25D41AB971E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="813" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="813" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data de prueba" sheetId="1" r:id="rId1"/>
     <sheet name="TC - Inicio de sesion" sheetId="2" r:id="rId2"/>
     <sheet name="TC - Filtro de productos" sheetId="3" r:id="rId3"/>
     <sheet name="TC - Carrito de compras" sheetId="5" r:id="rId4"/>
-    <sheet name="TC - Compra de productos" sheetId="4" r:id="rId5"/>
+    <sheet name="TC - Redes sociales(URL)" sheetId="6" r:id="rId5"/>
+    <sheet name="TC - Compra de productos" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
   <si>
     <t>Ambiente de prueba/URL</t>
   </si>
@@ -150,6 +151,57 @@
   </si>
   <si>
     <t>TC3</t>
+  </si>
+  <si>
+    <t>Validar filtro de productos: Por nombre</t>
+  </si>
+  <si>
+    <t>Validar filtro de productos: Por precio</t>
+  </si>
+  <si>
+    <t>Eliminar un producto del carrito de compras</t>
+  </si>
+  <si>
+    <t>Validar URL’s de las redes sociales de “Swag Labs”</t>
+  </si>
+  <si>
+    <t>URL de Redes Sociales</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
+    <t>https://twitter.com/saucelabs</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/saucelabs</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/sauce-labs/</t>
+  </si>
+  <si>
+    <t>Validar URL de Twitter</t>
+  </si>
+  <si>
+    <t>Validar URL de Linkedin</t>
+  </si>
+  <si>
+    <t>Validar URL de Facebook</t>
+  </si>
+  <si>
+    <t>La URL de Twitter debe ser: "https://twitter.com/saucelabs"</t>
+  </si>
+  <si>
+    <t>La URL de Facebook debe de ser: "https://www.facebook.com/saucelabs"</t>
+  </si>
+  <si>
+    <t>La URL de Linkedin debe ser "https://www.linkedin.com/company/sauce-labs/"</t>
   </si>
 </sst>
 </file>
@@ -231,13 +283,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,6 +316,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -574,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="G2" sqref="G2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,18 +644,27 @@
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="5"/>
+      <c r="G1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -607,34 +674,56 @@
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="G4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B339766F-73BC-40A5-9165-6054E3537316}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{E53A0EEA-7295-482E-80F3-082E624D3489}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{665702CA-7068-4144-9474-4A9F9B2C4162}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{4474D588-F925-4095-9E33-C6089D5AC521}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -643,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904F810-B7AD-41BE-8FC1-5BEEBBBF715B}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,32 +741,32 @@
     <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="48.21875" style="2" customWidth="1"/>
     <col min="7" max="7" width="61.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -691,12 +780,12 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D3" s="9">
+      <c r="D3" s="10">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -716,16 +805,16 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="12"/>
       <c r="G5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D6" s="9">
+      <c r="D6" s="10">
         <v>1</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -733,7 +822,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="11"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -745,16 +834,16 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="12"/>
       <c r="G8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D9" s="9">
+      <c r="D9" s="10">
         <v>1</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -762,7 +851,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="11"/>
+      <c r="E10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -774,7 +863,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,26 +877,26 @@
     <col min="7" max="7" width="69.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -819,9 +908,9 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -857,7 +946,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -917,26 +1006,26 @@
     <col min="7" max="7" width="69.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -948,9 +1037,9 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1028,6 +1117,123 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D775E97-D0AE-4B2B-BCFE-7948794070E5}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36" style="2" customWidth="1"/>
+    <col min="7" max="7" width="69.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="10">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="10">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D6" s="10">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="13"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" s="13"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="13"/>
+      <c r="H16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E22892-74CE-4E1A-9F86-BAF211CE1CD8}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -1046,26 +1252,26 @@
     <col min="7" max="7" width="69.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1079,7 +1285,7 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding compra de productos testcase
</commit_message>
<xml_diff>
--- a/solvex_testcases.xlsx
+++ b/solvex_testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rafael Mejia\solvex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D15886-1826-41CC-B489-25D41AB971E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5A67C3-71A6-42B6-B336-A216340D1F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="813" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="813" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data de prueba" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>Ambiente de prueba/URL</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Test Case</t>
-  </si>
-  <si>
-    <t>Realizar login con credenciales validas</t>
   </si>
   <si>
     <t>1. Tener link de la pagina : https://opensource-demo.orangehrmlive.com/
@@ -159,9 +156,6 @@
     <t>Validar filtro de productos: Por precio</t>
   </si>
   <si>
-    <t>Eliminar un producto del carrito de compras</t>
-  </si>
-  <si>
     <t>Validar URL’s de las redes sociales de “Swag Labs”</t>
   </si>
   <si>
@@ -202,6 +196,49 @@
   </si>
   <si>
     <t>La URL de Linkedin debe ser "https://www.linkedin.com/company/sauce-labs/"</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>Validar cierre de sesion</t>
+  </si>
+  <si>
+    <t>Hacer click en el menu de barras (esquina superior izquierda) y hacer click en el boton "Logout"</t>
+  </si>
+  <si>
+    <t>Se muestra la pagina de incio de sesion de "Swag Labs"</t>
+  </si>
+  <si>
+    <t>Realizar compra de 1 producto</t>
+  </si>
+  <si>
+    <t>1. Navegar hacia: https://www.saucedemo.com/
+2. Iniciar sesion con las credenciales (Usuario y Contraseña) validas de usuario.</t>
+  </si>
+  <si>
+    <t>Hacer click en el boton "Add to cart" de un producto y hacer click en el icono del carito (esquina superior derecha)</t>
+  </si>
+  <si>
+    <t>Se muestra el producto agregado al carrito de compras con el nombre, precio y descripcion del producto</t>
+  </si>
+  <si>
+    <t>Hacer click en el oton "Checkout"</t>
+  </si>
+  <si>
+    <t>Ingresar el nombre del usuario en el campo "First Name", el apellido del usuario en el campo "Last Name", el zipcode del usuario en el campo "Zip/Postal Code" y hacer click en el boton "Continue"</t>
+  </si>
+  <si>
+    <t>Se muestra la pantalla de "Checkout: Overview" con el precio total y los  detalles del producto</t>
+  </si>
+  <si>
+    <t>Se muestra la pantalla de "Checkout:Your Information" con campos: "First Name", "Last Name", Zip/Postal Code"</t>
+  </si>
+  <si>
+    <t>Hacer click en el boton "Finish"</t>
+  </si>
+  <si>
+    <t>Se muestra la pantalla de "Checkout: Complete" donde se muestra el mensaje "Thank you for your order!" confirmando la compra del producto</t>
   </si>
 </sst>
 </file>
@@ -283,7 +320,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,6 +356,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -635,7 +675,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:L4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +696,7 @@
       </c>
       <c r="D1" s="5"/>
       <c r="G1" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -675,10 +715,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -689,10 +729,10 @@
         <v>7</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -703,10 +743,10 @@
         <v>7</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -730,10 +770,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904F810-B7AD-41BE-8FC1-5BEEBBBF715B}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,16 +812,16 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -789,25 +829,25 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="12"/>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -815,10 +855,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -826,17 +866,17 @@
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="12"/>
       <c r="G8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -844,14 +884,51 @@
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D13" s="10">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -908,10 +985,10 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -919,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -927,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -935,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -946,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -957,7 +1034,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -968,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -979,7 +1056,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -989,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8F2398-C4AD-4C71-AAEA-48A83A072B82}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,13 +1077,13 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55" style="2" customWidth="1"/>
+    <col min="6" max="6" width="47.109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="69.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -1016,13 +1093,13 @@
       <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -1037,78 +1114,78 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" s="10">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" s="10">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1120,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D775E97-D0AE-4B2B-BCFE-7948794070E5}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1159,17 +1236,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1177,10 +1254,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1188,10 +1265,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1199,10 +1276,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1210,10 +1287,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1235,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E22892-74CE-4E1A-9F86-BAF211CE1CD8}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1246,9 +1323,9 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="52.44140625" style="14" customWidth="1"/>
     <col min="7" max="7" width="69.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1262,13 +1339,13 @@
       <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -1283,78 +1360,98 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D3" s="10">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D4">
+      <c r="E3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D5">
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D5" s="10">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D6" s="10">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Compra de productos testcases
</commit_message>
<xml_diff>
--- a/solvex_testcases.xlsx
+++ b/solvex_testcases.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rafael Mejia\solvex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5A67C3-71A6-42B6-B336-A216340D1F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122F3449-95A5-4D4F-AC3C-BF5E70A492E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="813" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="813" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data de prueba" sheetId="1" r:id="rId1"/>
     <sheet name="TC - Inicio de sesion" sheetId="2" r:id="rId2"/>
-    <sheet name="TC - Filtro de productos" sheetId="3" r:id="rId3"/>
-    <sheet name="TC - Carrito de compras" sheetId="5" r:id="rId4"/>
-    <sheet name="TC - Redes sociales(URL)" sheetId="6" r:id="rId5"/>
-    <sheet name="TC - Compra de productos" sheetId="4" r:id="rId6"/>
+    <sheet name="TC - Redes sociales(URL)" sheetId="6" r:id="rId3"/>
+    <sheet name="TC - Compra de productos" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Ambiente de prueba/URL</t>
   </si>
@@ -78,28 +76,6 @@
   </si>
   <si>
     <t>Test Case</t>
-  </si>
-  <si>
-    <t>1. Tener link de la pagina : https://opensource-demo.orangehrmlive.com/
-2. Tener el ID y la contraseña de usuario valido</t>
-  </si>
-  <si>
-    <t>Ingresar usuario en el campo "Username"</t>
-  </si>
-  <si>
-    <t>Ingresar contraseña en el campo "Password"</t>
-  </si>
-  <si>
-    <t>Hacer click en el boton "Login"</t>
-  </si>
-  <si>
-    <t>Realizar login con credenciales invalidas</t>
-  </si>
-  <si>
-    <t>Realizar busqueda de persona por ID</t>
-  </si>
-  <si>
-    <t>Otro</t>
   </si>
   <si>
     <t>Iniciar sesion con credenciales validas</t>
@@ -150,12 +126,6 @@
     <t>TC3</t>
   </si>
   <si>
-    <t>Validar filtro de productos: Por nombre</t>
-  </si>
-  <si>
-    <t>Validar filtro de productos: Por precio</t>
-  </si>
-  <si>
     <t>Validar URL’s de las redes sociales de “Swag Labs”</t>
   </si>
   <si>
@@ -239,6 +209,24 @@
   </si>
   <si>
     <t>Se muestra la pantalla de "Checkout: Complete" donde se muestra el mensaje "Thank you for your order!" confirmando la compra del producto</t>
+  </si>
+  <si>
+    <t>Cancelar la compra de un producto</t>
+  </si>
+  <si>
+    <t>Intentar realizar la compra de un producto sin ingresar los 'datos personales'</t>
+  </si>
+  <si>
+    <t>Hacer click en el boton "Cancelar"</t>
+  </si>
+  <si>
+    <t>Se muestra el dashboard de productos de Swag Labs</t>
+  </si>
+  <si>
+    <t>Dejar los campos de datos personales vacios y Hacer click en el boton "Continue"</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de error "Error: First Name is required" y no permite continuar con el flujo de compra del producto.</t>
   </si>
 </sst>
 </file>
@@ -696,7 +684,7 @@
       </c>
       <c r="D1" s="5"/>
       <c r="G1" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -715,10 +703,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -729,10 +717,10 @@
         <v>7</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -743,10 +731,10 @@
         <v>7</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +761,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,16 +800,16 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -829,25 +817,25 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E5" s="12"/>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -855,10 +843,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -866,17 +854,17 @@
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E8" s="12"/>
       <c r="G8" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -884,10 +872,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -895,16 +883,16 @@
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -912,10 +900,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -924,10 +912,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -936,8 +924,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E93F23-5D46-4A93-849D-BCD899850381}">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D775E97-D0AE-4B2B-BCFE-7948794070E5}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -945,265 +933,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8F2398-C4AD-4C71-AAEA-48A83A072B82}">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55" style="2" customWidth="1"/>
-    <col min="6" max="6" width="47.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="69.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D4" s="10">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D5" s="10">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D775E97-D0AE-4B2B-BCFE-7948794070E5}">
-  <dimension ref="A1:H16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
@@ -1237,16 +967,16 @@
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1254,10 +984,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1265,10 +995,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1276,10 +1006,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1287,10 +1017,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1310,23 +1040,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E22892-74CE-4E1A-9F86-BAF211CE1CD8}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="52.44140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="69.77734375" customWidth="1"/>
+    <col min="7" max="7" width="69.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1348,22 +1078,22 @@
       <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1371,10 +1101,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1382,10 +1112,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1393,10 +1123,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1404,54 +1134,115 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+        <v>59</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D10" s="10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="10">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D12" s="10">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D16" s="10">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D17" s="10">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>